<commit_message>
Added Runtime log relavant paths to Config
</commit_message>
<xml_diff>
--- a/Data/Config - Copy.xlsx
+++ b/Data/Config - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://appriver3651001021-my.sharepoint.com/personal/calypso_inpwrinc_com/Documents/Documents/UiPath/InPwr.Finance.AccountsPayable.Dispatcher/InPwr.Finance.AccountsPayable.Dispatcher/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CoEBusinessAnalystIC\Documents\InPwr.Finance.AccountsPayable.Dispatcher\AP_Dispatcher_Common\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{1F61DB99-DFAD-4A46-BA3B-D4C27AAD35DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49C76559-D3C4-48F9-B4D3-381CA79B2967}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723754E4-E7DC-45F5-BF15-C9602CFCA2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
   <si>
     <t>Name</t>
   </si>
@@ -193,9 +193,6 @@
 Support Team</t>
   </si>
   <si>
-    <t>The delay or time interval before retrying the action for the AP Invoice Mailbox connection.</t>
-  </si>
-  <si>
     <t>AP Invoice Mail account name.</t>
   </si>
   <si>
@@ -211,85 +208,28 @@
     <t>32fd5246-0465-417c-bed3-518983955cb3</t>
   </si>
   <si>
-    <t>Inbox\AP INVOICE ENTRY - CoE</t>
-  </si>
-  <si>
-    <t>VendorEmailDomain</t>
-  </si>
-  <si>
-    <t>Inbox\AP INVOICE ENTRY - CoE\Excluded</t>
-  </si>
-  <si>
     <t>Document understanding Queue name which is created in the Orchestrator Queue folder.</t>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name.</t>
   </si>
   <si>
-    <t>The number of retry attempts for connecting the AP Invoice mailbox.</t>
-  </si>
-  <si>
-    <t>Time out for Microsoft office 365 Application scope (in seconds)</t>
-  </si>
-  <si>
-    <t>The maximum number of emails to be retrieved from the AP Invoice Input folder.</t>
-  </si>
-  <si>
-    <t>The Input mail folder name to retrieve the incoming emails from AP Invoice mailbox.</t>
-  </si>
-  <si>
-    <t>The Entity name in Data service which holds the TEMP Vendor master list.</t>
-  </si>
-  <si>
-    <t>Field or column name that holds the vendor name details in the Entity.</t>
-  </si>
-  <si>
-    <t>Field or column name that holds the vendor Domain details in the Entity.</t>
-  </si>
-  <si>
     <t>Temp queue mail folder name for the AP Invoice mailbox.</t>
   </si>
   <si>
     <t>Manual review mail folder name for the AP Invoice mailbox.</t>
   </si>
   <si>
-    <t>Exlusion mail folder name for the AP Invoice mailbox.</t>
-  </si>
-  <si>
-    <t>Refresh token for the Data Service within the API scope.</t>
-  </si>
-  <si>
-    <t>Client Secret Id for the Data Service within the API scope.</t>
-  </si>
-  <si>
     <t>Initial_Staging</t>
   </si>
   <si>
-    <t>ERPVendorType</t>
-  </si>
-  <si>
-    <t>ERPVendorName</t>
-  </si>
-  <si>
-    <t>InPwr domain name in lower case.</t>
-  </si>
-  <si>
     <t>The number of retry attempts for connecting the Network share drive.</t>
   </si>
   <si>
     <t>The delay or time interval before retrying the action for the Network share drive.</t>
   </si>
   <si>
-    <t>The number of retry attempts for queue activities.</t>
-  </si>
-  <si>
-    <t>The delay or time interval before retrying the action for the queue activities.</t>
-  </si>
-  <si>
     <t>PDF attachment folder path where file needs to be downloaded.</t>
-  </si>
-  <si>
-    <t>Regex pattern for Invoice Subject validation.</t>
   </si>
   <si>
     <t>Dear All,
@@ -301,45 +241,9 @@
 Support Team</t>
   </si>
   <si>
-    <t>Data\Temp\</t>
-  </si>
-  <si>
-    <t>@inpwrinc.com</t>
-  </si>
-  <si>
-    <t>^(.*?)(?=__?INVOICE)</t>
-  </si>
-  <si>
     <t>Finance/Accounts Payable/DISPATCHER</t>
   </si>
   <si>
-    <t>Unable to determine source vendor from email domain.</t>
-  </si>
-  <si>
-    <t>Behavior</t>
-  </si>
-  <si>
-    <t>as extracted</t>
-  </si>
-  <si>
-    <t>Email domain is Excluded.</t>
-  </si>
-  <si>
-    <t>Mail Subject is empty hence unable to fetch vendor name.</t>
-  </si>
-  <si>
-    <t>Unable to determine source vendor from email subject line.</t>
-  </si>
-  <si>
-    <t>Email Subject is Excluded.</t>
-  </si>
-  <si>
-    <t>AP_ExtractionQueue_RetryCount</t>
-  </si>
-  <si>
-    <t>AP_ExtractionQueue_RetryInterval</t>
-  </si>
-  <si>
     <t>AP_ExtractionQueue_Folder</t>
   </si>
   <si>
@@ -349,254 +253,134 @@
     <t>AP_O365_MailAccount</t>
   </si>
   <si>
-    <t>AP_O365_RetryCount</t>
-  </si>
-  <si>
-    <t>AP_O365_RetryInterval</t>
-  </si>
-  <si>
     <t>AP_O365_TenantId</t>
   </si>
   <si>
-    <t>AP_O365_Timeout</t>
-  </si>
-  <si>
-    <t>AP_O365_MailReadLimit</t>
-  </si>
-  <si>
-    <t>Queued_TEMP</t>
-  </si>
-  <si>
     <t>AP_SharedDrive_RetryCount</t>
   </si>
   <si>
-    <t>AP_O365_MailFolder_Input</t>
-  </si>
-  <si>
     <t>AP_O365_MailFolder_ManualReview</t>
   </si>
   <si>
-    <t>AP_O365_MailFolder_Excluded</t>
-  </si>
-  <si>
     <t>AP_O365_MailFolder_Queued</t>
   </si>
   <si>
     <t>AP_SharedDrive_RetryInterval</t>
   </si>
   <si>
+    <t>AP_SharedDrive_RuntimeLog_Success</t>
+  </si>
+  <si>
+    <t>AP_SharedDrive_Attachment</t>
+  </si>
+  <si>
+    <t>AP_SharedDrive_Runtime_SheetName</t>
+  </si>
+  <si>
+    <t>AP_O365_Application</t>
+  </si>
+  <si>
+    <t>Finance/Accounts Payable/EXTRACTION/&lt;VendorType&gt;</t>
+  </si>
+  <si>
+    <t>Inbox\AP INVOICE ENTRY - CoE\Queued\&lt;VendorType&gt;</t>
+  </si>
+  <si>
+    <t>AP_ExceptionLogMessage_DownloadPDF</t>
+  </si>
+  <si>
+    <t>Unable to download Email Attachment.</t>
+  </si>
+  <si>
+    <t>AP_MailAddress</t>
+  </si>
+  <si>
+    <t>AP_SharedDrive_MappingScript_Flag</t>
+  </si>
+  <si>
+    <t>AP_SharedDrive_UNC</t>
+  </si>
+  <si>
+    <t>\\inpwrautomation.file.core.windows.net\automation\</t>
+  </si>
+  <si>
+    <t>Actual share drive path and IP address are not allowed.</t>
+  </si>
+  <si>
+    <t>Accepts only an Boolean (TRUE or FALSE).</t>
+  </si>
+  <si>
+    <t>AP_SharedDrive_MappingDriveLetter</t>
+  </si>
+  <si>
+    <t>Drive letter should not already be mapped in the system.</t>
+  </si>
+  <si>
+    <t>AP_SharedDrive_ActutalMappingPath</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>AP_Local_MasterFolder</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>&lt;VendorType&gt;_DU_Queue</t>
+  </si>
+  <si>
+    <t>&lt;DriveLetter&gt;:\RPA</t>
+  </si>
+  <si>
+    <t>&lt;DriveLetter&gt;:\RPA\APInvoice\&lt;TenantName&gt;\PDF\&lt;VendorType&gt;\&lt;CurrentDate&gt;\</t>
+  </si>
+  <si>
+    <t>APInvoice.Dispatcher</t>
+  </si>
+  <si>
+    <t>Finance/Accounts Payable</t>
+  </si>
+  <si>
+    <t>Mail Address to send exception notification.</t>
+  </si>
+  <si>
+    <t>AP_O365_Application_AssetFolder</t>
+  </si>
+  <si>
+    <t>Success Runtime Staging Log excel folder path.</t>
+  </si>
+  <si>
+    <t>Initial Sheet name for Runtime Staging log excel file.</t>
+  </si>
+  <si>
+    <t>mercury@inpwrinc.com</t>
+  </si>
+  <si>
+    <t>AP_DispatcherQueue_Folder</t>
+  </si>
+  <si>
+    <t>calypso@inpwrinc.com</t>
+  </si>
+  <si>
+    <t>C:\RPA\</t>
+  </si>
+  <si>
+    <t>&lt;DriveLetter&gt;:\RPA\APInvoice\&lt;TenantName&gt;\Log\&lt;VendorType&gt;\&lt;CurrentDate&gt;_SuccessLog.xlsx</t>
+  </si>
+  <si>
     <t>AP_SharedDrive_RuntimeLog_Exception</t>
   </si>
   <si>
-    <t>AP_SharedDrive_RuntimeLog_Template</t>
-  </si>
-  <si>
-    <t>AP_SharedDrive_RuntimeLog_Success</t>
-  </si>
-  <si>
-    <t>AP_SharedDrive_Attachment</t>
-  </si>
-  <si>
-    <t>AP_DataService_EntityName</t>
-  </si>
-  <si>
-    <t>AP_DataService_FieldName_Domain</t>
-  </si>
-  <si>
-    <t>AP_DataService_FieldName_VendorType</t>
-  </si>
-  <si>
-    <t>AP_DataService_FieldName_VendorName</t>
-  </si>
-  <si>
-    <t>AP_DataService_PostProcessing_FilterValue</t>
-  </si>
-  <si>
-    <t>AP_DataService_PostProcessing_FilterName</t>
-  </si>
-  <si>
-    <t>AP_ExceptionLogMessage_Domain</t>
-  </si>
-  <si>
-    <t>AP_ExceptionLogMessage_DomainExcluded</t>
-  </si>
-  <si>
-    <t>AP_ExceptionLogMessage_SubjectMissed</t>
-  </si>
-  <si>
-    <t>AP_ExceptionLogMessage_Subject</t>
-  </si>
-  <si>
-    <t>AP_ExceptionLogMessage_SubjectExcluded</t>
-  </si>
-  <si>
-    <t>AP_MailValidation_InPwrDomainName</t>
-  </si>
-  <si>
-    <t>AP_MailValidation_InvoiceSubjectRegex</t>
-  </si>
-  <si>
-    <t>AP_SaveEmail_LocalFolder</t>
-  </si>
-  <si>
-    <t>AP_SharedDrive_Runtime_SheetName</t>
-  </si>
-  <si>
-    <t>AP_O365_Application</t>
-  </si>
-  <si>
-    <t>AP_DataService_API</t>
-  </si>
-  <si>
-    <t>AP_DataService_RefreshToken</t>
-  </si>
-  <si>
-    <t>Finance/Accounts Payable/EXTRACTION/&lt;VendorType&gt;</t>
-  </si>
-  <si>
-    <t>Inbox\AP INVOICE ENTRY - CoE\Queued\&lt;VendorType&gt;</t>
-  </si>
-  <si>
-    <t>Field or Column name that needs to consider for Post processing rule from the Entity.</t>
-  </si>
-  <si>
-    <t>Field Value that needs to removed in Post processing rule from the Entity.</t>
-  </si>
-  <si>
-    <t>Local folder path for Saving mail.</t>
-  </si>
-  <si>
-    <t>Exception log message for Subject not found in mail validation.</t>
-  </si>
-  <si>
-    <t>Exception log message for Domain not found in Entity during mail validation.</t>
-  </si>
-  <si>
-    <t>Exception log message for Excluded Domain in Entity during mail validation.</t>
-  </si>
-  <si>
-    <t>Exception log message for Subject not found in Entity during mail validation.</t>
-  </si>
-  <si>
-    <t>Exception log message for Excluded Subject in Entity during mail validation.</t>
-  </si>
-  <si>
-    <t>No PDF Attachment available.</t>
-  </si>
-  <si>
-    <t>AP_ExceptionLogMessage_PDFAttachment</t>
-  </si>
-  <si>
-    <t>AP_ExceptionLogMessage_DownloadPDF</t>
-  </si>
-  <si>
-    <t>Unable to download Email Attachment.</t>
-  </si>
-  <si>
-    <t>AP_MailAddress</t>
-  </si>
-  <si>
-    <t>AP_SharedDrive_MappingScript_Flag</t>
-  </si>
-  <si>
-    <t>AP_KillApplication_Collection</t>
-  </si>
-  <si>
-    <t>EXCEL|msedge</t>
-  </si>
-  <si>
-    <t>AP_SharedDrive_UNC</t>
-  </si>
-  <si>
-    <t>\\inpwrautomation.file.core.windows.net\automation\</t>
-  </si>
-  <si>
-    <t>Actual share drive path and IP address are not allowed.</t>
-  </si>
-  <si>
-    <t>Accepts only an Boolean (TRUE or FALSE).</t>
-  </si>
-  <si>
-    <t>AP_SharedDrive_MappingDriveLetter</t>
-  </si>
-  <si>
-    <t>Drive letter should not already be mapped in the system.</t>
-  </si>
-  <si>
-    <t>AP_SharedDrive_ActutalMappingPath</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>AP_Local_MasterFolder</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>&lt;VendorType&gt;_DU_Queue</t>
-  </si>
-  <si>
-    <t>&lt;DriveLetter&gt;:\RPA</t>
-  </si>
-  <si>
-    <t>&lt;DriveLetter&gt;:\RPA\APInvoice\&lt;TenantName&gt;\PDF\&lt;VendorType&gt;\&lt;CurrentDate&gt;\</t>
-  </si>
-  <si>
-    <t>&lt;DriveLetter&gt;:\RPA\APInvoice\&lt;TenantName&gt;\Log\&lt;VendorType&gt;\</t>
-  </si>
-  <si>
-    <t>&lt;DriveLetter&gt;:\RPA\APInvoice\&lt;TenantName&gt;\Log\Log_Template.xlsx</t>
-  </si>
-  <si>
-    <t>&lt;DriveLetter&gt;:\RPA\APInvoice\&lt;TenantName&gt;\Log\Exception\</t>
-  </si>
-  <si>
-    <t>APInvoice.Dispatcher</t>
-  </si>
-  <si>
-    <t>Finance/Accounts Payable</t>
-  </si>
-  <si>
-    <t>Mail Address to send exception notification.</t>
-  </si>
-  <si>
-    <t>AP_O365_Application_AssetFolder</t>
-  </si>
-  <si>
-    <t>Exception Runtime Staging Log excel folder path.</t>
-  </si>
-  <si>
-    <t>Success Runtime Staging Log excel folder path.</t>
-  </si>
-  <si>
-    <t>Template for Runtime Staging Log excel file path.</t>
-  </si>
-  <si>
-    <t>Initial Sheet name for Runtime Staging log excel file.</t>
-  </si>
-  <si>
-    <t>&lt;ProjectLocation&gt;\RPA\</t>
-  </si>
-  <si>
-    <t>mercury@inpwrinc.com</t>
-  </si>
-  <si>
-    <t>FinanceAPVendorMasterListPOMaterial</t>
-  </si>
-  <si>
-    <t>AP_DispatcherQueue_Folder</t>
-  </si>
-  <si>
-    <t>calypso@inpwrinc.com</t>
+    <t>&lt;DriveLetter&gt;:\RPA\APInvoice\&lt;TenantName&gt;\Log\Exception\&lt;VendorType&gt;\&lt;CurrentDate&gt;_ExceptionLog.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -628,12 +412,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -662,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -696,9 +474,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -708,10 +483,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1027,9 +798,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1002"/>
+  <dimension ref="A1:Y974"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -1079,10 +850,10 @@
         <v>20</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>172</v>
+        <v>100</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1090,10 +861,10 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>107</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -1102,10 +873,10 @@
     </row>
     <row r="6" spans="1:25" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>138</v>
+        <v>69</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>27</v>
@@ -1113,495 +884,243 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>166</v>
+        <v>70</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="12">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:25" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="12">
-        <v>30</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="14.25" customHeight="1">
-      <c r="C10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="11">
-        <v>3</v>
+      <c r="A11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="11">
-        <v>30</v>
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" s="11">
-        <v>60000</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:25" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>60</v>
+        <v>86</v>
+      </c>
+      <c r="B15" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>139</v>
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>112</v>
+      <c r="A17" t="s">
+        <v>93</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>62</v>
+        <v>87</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
+        <v>73</v>
+      </c>
+      <c r="B19" s="12">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>175</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>173</v>
+        <v>76</v>
+      </c>
+      <c r="B20" s="12">
+        <v>30</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B21" s="11"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="A22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>163</v>
+      <c r="A23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>161</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>167</v>
+        <v>63</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>161</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>156</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>158</v>
-      </c>
+      <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" s="12">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>81</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" s="12">
-        <v>30</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>176</v>
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>164</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" t="s">
-        <v>136</v>
-      </c>
-      <c r="B42" t="s">
-        <v>136</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" t="s">
-        <v>126</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A45" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A46" t="s">
-        <v>128</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A47" t="s">
-        <v>129</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A48" t="s">
-        <v>130</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C48" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A49" t="s">
-        <v>149</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A50" t="s">
-        <v>150</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A52" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1">
-      <c r="A53" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A55" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A57" t="s">
-        <v>154</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="59" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -2512,34 +2031,6 @@
     <row r="972" ht="14.25" customHeight="1"/>
     <row r="973" ht="14.25" customHeight="1"/>
     <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3712,10 +3203,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z978"/>
+  <dimension ref="A1:Z976"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3763,75 +3254,49 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" t="s">
-        <v>137</v>
+      <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>103</v>
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" t="s">
-        <v>55</v>
+        <v>96</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" t="s">
-        <v>108</v>
+      <c r="A4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4802,8 +4267,6 @@
     <row r="974" ht="14.25" customHeight="1"/>
     <row r="975" ht="14.25" customHeight="1"/>
     <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4812,10 +4275,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A045ED-89B2-46F5-87BB-9D73B35EE197}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4823,13 +4286,12 @@
     <col min="1" max="1" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="22.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="8"/>
+    <col min="4" max="4" width="26.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
@@ -4840,39 +4302,27 @@
         <v>40</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="285">
+    <row r="2" spans="1:5" ht="285">
       <c r="A2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>87</v>
+      <c r="E2" s="13" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -4926,8 +4376,8 @@
       <c r="B2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>181</v>
+      <c r="C2" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>50</v>

</xml_diff>